<commit_message>
arrumando a rota principal (sua turma)
</commit_message>
<xml_diff>
--- a/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
+++ b/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeusRepositorios\frequencia.simples\arquivos_diversos\extras_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01319988-EDA2-47B3-829E-B880BE3A467B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BA389F-9434-4C0C-9C09-874266B4EC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="coisas a fazer" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
   <si>
     <t>FUNCIONALIDADE</t>
   </si>
@@ -173,13 +174,37 @@
   </si>
   <si>
     <t>Criar um sistema para que, quando o catequista logar no sistema, e sua data de aniversário for no dia ou tiver passado pelo menos 5 dias de sua data de aniversário, apareça um pop-up desejando felicitações pela sua data de nascimento</t>
+  </si>
+  <si>
+    <t>Coisas que ainda faltam serem feitas no projeto</t>
+  </si>
+  <si>
+    <t>Terminar a página de Inicio (História da Igreja e da Pastoral, e pensar e projetar como será a página)</t>
+  </si>
+  <si>
+    <t>Colocar a Quant. De crismandos no card de grupos da crisma (pagina Grupos)</t>
+  </si>
+  <si>
+    <t>Criar página de perfi, com as informações do usuário (nele terá a opção de editar infor., foto de perfil (?), senha e email)</t>
+  </si>
+  <si>
+    <t>Página p/ relatar bugs</t>
+  </si>
+  <si>
+    <t>Mehorar o digitamento das informações (por exemplo: permitir onde é para aceitar numero, só aceite numero e já fique formatado)</t>
+  </si>
+  <si>
+    <t>Modificar algumas coisas no banco de dados (fazer melhoramentos e adicionar colunas ( adicionar colunas em "crismandos" como por exemplo estado civil, se possui filhos, cidade, etc))</t>
+  </si>
+  <si>
+    <t>Melhorar ou modificar o sistema de login e cadastro de catequista</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +227,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -217,7 +250,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -240,11 +273,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -255,9 +346,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -269,6 +357,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,49 +684,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="4" width="36.5546875" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="6" customWidth="1"/>
     <col min="6" max="6" width="36.5546875" customWidth="1"/>
     <col min="7" max="7" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="2:6" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -630,7 +740,7 @@
       <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -647,7 +757,7 @@
       <c r="D4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -664,7 +774,7 @@
       <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -681,7 +791,7 @@
       <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -698,7 +808,7 @@
       <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -715,7 +825,7 @@
       <c r="D8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -732,7 +842,7 @@
       <c r="D9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -749,7 +859,7 @@
       <c r="D10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -766,7 +876,7 @@
       <c r="D11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -783,7 +893,7 @@
       <c r="D12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -800,7 +910,7 @@
       <c r="D13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -817,10 +927,10 @@
       <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -834,10 +944,10 @@
       <c r="D16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -851,10 +961,10 @@
       <c r="D17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -868,10 +978,10 @@
       <c r="D18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -885,10 +995,10 @@
       <c r="D19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -902,10 +1012,10 @@
       <c r="D20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -923,4 +1033,99 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700300DC-6034-43CC-8CAB-6840AC52BDFC}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="51.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
editando a pagina inicio
</commit_message>
<xml_diff>
--- a/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
+++ b/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeusRepositorios\frequencia.simples\arquivos_diversos\extras_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BA389F-9434-4C0C-9C09-874266B4EC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D1A615-AD87-4216-9C23-A26B6318E6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -236,7 +236,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,6 +246,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -380,6 +386,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1037,31 +1047,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700300DC-6034-43CC-8CAB-6840AC52BDFC}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="51.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="16" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C2" s="17">
+        <v>45780</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -1069,7 +1083,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -1077,7 +1091,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -1085,7 +1099,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -1093,7 +1107,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -1101,7 +1115,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -1109,19 +1123,19 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
criando função de enviar email ao logar
</commit_message>
<xml_diff>
--- a/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
+++ b/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeusRepositorios\frequencia.simples\arquivos_diversos\extras_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D1A615-AD87-4216-9C23-A26B6318E6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36812BC6-EEDF-42AE-A811-FBDC5AAD2073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
   <si>
     <t>FUNCIONALIDADE</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Melhorar ou modificar o sistema de login e cadastro de catequista</t>
+  </si>
+  <si>
+    <t>Criar a rota e paginas para editar informações de um grupo</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1053,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,7 +1083,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1088,46 +1091,48 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
+      <c r="A9" s="15">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>

</xml_diff>

<commit_message>
criando opção de relatar bugs
</commit_message>
<xml_diff>
--- a/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
+++ b/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeusRepositorios\frequencia.simples\arquivos_diversos\extras_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36812BC6-EEDF-42AE-A811-FBDC5AAD2073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB2C30C-3F41-4279-86E6-59530D829F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -239,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,6 +258,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -344,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -393,6 +399,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1053,7 +1062,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1098,8 +1107,11 @@
       <c r="A5" s="15">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="18" t="s">
         <v>53</v>
+      </c>
+      <c r="C5" s="17">
+        <v>45781</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
adicionando colunas nas infor's de crismandos
</commit_message>
<xml_diff>
--- a/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
+++ b/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeusRepositorios\frequencia.simples\arquivos_diversos\extras_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB2C30C-3F41-4279-86E6-59530D829F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D1C11B-7553-4774-AB7E-71573DA7BEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1062,7 +1062,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1126,8 +1126,11 @@
       <c r="A7" s="15">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="18" t="s">
         <v>55</v>
+      </c>
+      <c r="C7" s="17">
+        <v>45782</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
adc. quant. de crismandos nos cards
</commit_message>
<xml_diff>
--- a/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
+++ b/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeusRepositorios\frequencia.simples\arquivos_diversos\extras_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D1C11B-7553-4774-AB7E-71573DA7BEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0818E93B-F434-4DDF-B098-5BDFA5643E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
   <si>
     <t>FUNCIONALIDADE</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Criar a rota e paginas para editar informações de um grupo</t>
+  </si>
+  <si>
+    <t>Aprender a fazer backup do banco de dados</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1065,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1137,8 +1140,11 @@
       <c r="A8" s="15">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="18" t="s">
         <v>51</v>
+      </c>
+      <c r="C8" s="17">
+        <v>45784</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1147,6 +1153,14 @@
       </c>
       <c r="B9" s="8" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
botando mascara em input e resolvendo bugs
</commit_message>
<xml_diff>
--- a/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
+++ b/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeusRepositorios\frequencia.simples\arquivos_diversos\extras_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0818E93B-F434-4DDF-B098-5BDFA5643E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6A8C58-0B56-4C7D-B97F-8A93F46C6CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
   <si>
     <t>FUNCIONALIDADE</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>Aprender a fazer backup do banco de dados</t>
+  </si>
+  <si>
+    <t>Fazer a divisão do banco de dados de testes e de produção</t>
+  </si>
+  <si>
+    <t>Deixar o projeto online com base de dados ativa</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1071,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,10 +1170,20 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
+      <c r="A11" s="15">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
+      <c r="A12" s="15">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>

</xml_diff>

<commit_message>
editando bug do avatar
</commit_message>
<xml_diff>
--- a/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
+++ b/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeusRepositorios\frequencia.simples\arquivos_diversos\extras_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6A8C58-0B56-4C7D-B97F-8A93F46C6CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2823BDE7-968E-4DFD-9BE9-491A95783447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1071,7 +1071,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,8 +1127,11 @@
       <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="18" t="s">
         <v>54</v>
+      </c>
+      <c r="C6" s="17">
+        <v>45786</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
criando a opção de editar infor dos grupos
</commit_message>
<xml_diff>
--- a/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
+++ b/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeusRepositorios\frequencia.simples\arquivos_diversos\extras_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2823BDE7-968E-4DFD-9BE9-491A95783447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D35B65C-2464-42C9-8FC1-27DA38209502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
   <si>
     <t>FUNCIONALIDADE</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Deixar o projeto online com base de dados ativa</t>
+  </si>
+  <si>
+    <t>Implementar o Flask-WTF, mas só depois da 1ºVersão</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700300DC-6034-43CC-8CAB-6840AC52BDFC}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1191,6 +1194,14 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="15">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
resolvendo bug de logout
</commit_message>
<xml_diff>
--- a/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
+++ b/arquivos_diversos/extras_files/cronograma_funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeusRepositorios\frequencia.simples\arquivos_diversos\extras_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D35B65C-2464-42C9-8FC1-27DA38209502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BCB3FF-B491-4770-AD62-E1CC976556EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1074,7 +1074,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1163,8 +1163,11 @@
       <c r="A9" s="15">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="18" t="s">
         <v>57</v>
+      </c>
+      <c r="C9" s="17">
+        <v>45787</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>